<commit_message>
commit - fetch data from DB and generate excel file
</commit_message>
<xml_diff>
--- a/book.xlsx
+++ b/book.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G101"/>
+  <dimension ref="A1:H101"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -402,16 +402,19 @@
       <c r="G1" t="str">
         <v>price</v>
       </c>
+      <c r="H1" t="str">
+        <v>__v</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="str">
-        <v>3/27/2018</v>
+        <v>2018-03-26T18:30:00.000Z</v>
       </c>
       <c r="C2" t="str">
-        <v>5/24/2019</v>
+        <v>2019-05-23T18:30:00.000Z</v>
       </c>
       <c r="D2" t="str">
         <v>28058 Hazelcrest Center</v>
@@ -424,6 +427,9 @@
       </c>
       <c r="G2">
         <v>376</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -431,10 +437,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="str">
-        <v>6/14/2018</v>
+        <v>2018-06-13T18:30:00.000Z</v>
       </c>
       <c r="C3" t="str">
-        <v>11/14/2018</v>
+        <v>2018-11-13T18:30:00.000Z</v>
       </c>
       <c r="D3" t="str">
         <v>6205 Shopko Court</v>
@@ -447,6 +453,9 @@
       </c>
       <c r="G3">
         <v>285</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -454,10 +463,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="str">
-        <v>9/4/2018</v>
+        <v>2018-09-03T18:30:00.000Z</v>
       </c>
       <c r="C4" t="str">
-        <v>2/21/2019</v>
+        <v>2019-02-20T18:30:00.000Z</v>
       </c>
       <c r="D4" t="str">
         <v>49 Spenser Plaza</v>
@@ -470,6 +479,9 @@
       </c>
       <c r="G4">
         <v>318</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -477,10 +489,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="str">
-        <v>1/20/2019</v>
+        <v>2019-01-19T18:30:00.000Z</v>
       </c>
       <c r="C5" t="str">
-        <v>3/25/2019</v>
+        <v>2019-03-24T18:30:00.000Z</v>
       </c>
       <c r="D5" t="str">
         <v>49596 Aberg Point</v>
@@ -493,6 +505,9 @@
       </c>
       <c r="G5">
         <v>290</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -500,10 +515,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="str">
-        <v>1/20/2018</v>
+        <v>2018-01-19T18:30:00.000Z</v>
       </c>
       <c r="C6" t="str">
-        <v>12/31/2018</v>
+        <v>2018-12-30T18:30:00.000Z</v>
       </c>
       <c r="D6" t="str">
         <v>10667 Blaine Drive</v>
@@ -516,6 +531,9 @@
       </c>
       <c r="G6">
         <v>200</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -523,10 +541,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="str">
-        <v>9/1/2018</v>
+        <v>2018-08-31T18:30:00.000Z</v>
       </c>
       <c r="C7" t="str">
-        <v>5/2/2018</v>
+        <v>2018-05-01T18:30:00.000Z</v>
       </c>
       <c r="D7" t="str">
         <v>9692 Karstens Terrace</v>
@@ -539,6 +557,9 @@
       </c>
       <c r="G7">
         <v>101</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -546,10 +567,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="str">
-        <v>3/23/2019</v>
+        <v>2019-03-22T18:30:00.000Z</v>
       </c>
       <c r="C8" t="str">
-        <v>5/19/2019</v>
+        <v>2019-05-18T18:30:00.000Z</v>
       </c>
       <c r="D8" t="str">
         <v>3 Stone Corner Place</v>
@@ -562,6 +583,9 @@
       </c>
       <c r="G8">
         <v>270</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -569,10 +593,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="str">
-        <v>9/21/2018</v>
+        <v>2018-09-20T18:30:00.000Z</v>
       </c>
       <c r="C9" t="str">
-        <v>10/4/2018</v>
+        <v>2018-10-03T18:30:00.000Z</v>
       </c>
       <c r="D9" t="str">
         <v>5 Prairieview Drive</v>
@@ -585,6 +609,9 @@
       </c>
       <c r="G9">
         <v>285</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -592,10 +619,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="str">
-        <v>11/5/2018</v>
+        <v>2018-11-04T18:30:00.000Z</v>
       </c>
       <c r="C10" t="str">
-        <v>3/19/2019</v>
+        <v>2019-03-18T18:30:00.000Z</v>
       </c>
       <c r="D10" t="str">
         <v>08 Melrose Hill</v>
@@ -608,6 +635,9 @@
       </c>
       <c r="G10">
         <v>339</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -615,10 +645,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="str">
-        <v>3/11/2019</v>
+        <v>2019-03-10T18:30:00.000Z</v>
       </c>
       <c r="C11" t="str">
-        <v>5/16/2019</v>
+        <v>2019-05-15T18:30:00.000Z</v>
       </c>
       <c r="D11" t="str">
         <v>6325 Onsgard Drive</v>
@@ -631,6 +661,9 @@
       </c>
       <c r="G11">
         <v>93</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -638,10 +671,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="str">
-        <v>3/16/2018</v>
+        <v>2018-03-15T18:30:00.000Z</v>
       </c>
       <c r="C12" t="str">
-        <v>9/29/2018</v>
+        <v>2018-09-28T18:30:00.000Z</v>
       </c>
       <c r="D12" t="str">
         <v>54502 Fremont Drive</v>
@@ -654,6 +687,9 @@
       </c>
       <c r="G12">
         <v>380</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -661,10 +697,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="str">
-        <v>7/10/2018</v>
+        <v>2018-07-09T18:30:00.000Z</v>
       </c>
       <c r="C13" t="str">
-        <v>12/24/2018</v>
+        <v>2018-12-23T18:30:00.000Z</v>
       </c>
       <c r="D13" t="str">
         <v>2 Warbler Street</v>
@@ -677,6 +713,9 @@
       </c>
       <c r="G13">
         <v>276</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -684,10 +723,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="str">
-        <v>5/7/2018</v>
+        <v>2018-05-06T18:30:00.000Z</v>
       </c>
       <c r="C14" t="str">
-        <v>11/21/2018</v>
+        <v>2018-11-20T18:30:00.000Z</v>
       </c>
       <c r="D14" t="str">
         <v>16679 Doe Crossing Road</v>
@@ -700,6 +739,9 @@
       </c>
       <c r="G14">
         <v>287</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -707,10 +749,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="str">
-        <v>12/24/2018</v>
+        <v>2018-12-23T18:30:00.000Z</v>
       </c>
       <c r="C15" t="str">
-        <v>6/14/2018</v>
+        <v>2018-06-13T18:30:00.000Z</v>
       </c>
       <c r="D15" t="str">
         <v>21 Dottie Hill</v>
@@ -723,6 +765,9 @@
       </c>
       <c r="G15">
         <v>405</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
       </c>
     </row>
     <row r="16">
@@ -730,10 +775,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="str">
-        <v>2/15/2018</v>
+        <v>2018-02-14T18:30:00.000Z</v>
       </c>
       <c r="C16" t="str">
-        <v>9/21/2018</v>
+        <v>2018-09-20T18:30:00.000Z</v>
       </c>
       <c r="D16" t="str">
         <v>73 Maple Wood Junction</v>
@@ -746,6 +791,9 @@
       </c>
       <c r="G16">
         <v>194</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -753,10 +801,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="str">
-        <v>7/4/2018</v>
+        <v>2018-07-03T18:30:00.000Z</v>
       </c>
       <c r="C17" t="str">
-        <v>12/17/2018</v>
+        <v>2018-12-16T18:30:00.000Z</v>
       </c>
       <c r="D17" t="str">
         <v>72 Barby Junction</v>
@@ -769,6 +817,9 @@
       </c>
       <c r="G17">
         <v>352</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -776,10 +827,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="str">
-        <v>4/26/2018</v>
+        <v>2018-04-25T18:30:00.000Z</v>
       </c>
       <c r="C18" t="str">
-        <v>6/17/2018</v>
+        <v>2018-06-16T18:30:00.000Z</v>
       </c>
       <c r="D18" t="str">
         <v>7763 Hagan Avenue</v>
@@ -792,6 +843,9 @@
       </c>
       <c r="G18">
         <v>120</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
       </c>
     </row>
     <row r="19">
@@ -799,10 +853,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="str">
-        <v>1/27/2018</v>
+        <v>2018-01-26T18:30:00.000Z</v>
       </c>
       <c r="C19" t="str">
-        <v>6/11/2019</v>
+        <v>2019-06-10T18:30:00.000Z</v>
       </c>
       <c r="D19" t="str">
         <v>4313 Roxbury Plaza</v>
@@ -815,6 +869,9 @@
       </c>
       <c r="G19">
         <v>120</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
       </c>
     </row>
     <row r="20">
@@ -822,10 +879,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="str">
-        <v>12/28/2018</v>
+        <v>2018-12-27T18:30:00.000Z</v>
       </c>
       <c r="C20" t="str">
-        <v>3/9/2019</v>
+        <v>2019-03-08T18:30:00.000Z</v>
       </c>
       <c r="D20" t="str">
         <v>34 Karstens Point</v>
@@ -838,6 +895,9 @@
       </c>
       <c r="G20">
         <v>225</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
       </c>
     </row>
     <row r="21">
@@ -845,10 +905,10 @@
         <v>20</v>
       </c>
       <c r="B21" t="str">
-        <v>8/10/2018</v>
+        <v>2018-08-09T18:30:00.000Z</v>
       </c>
       <c r="C21" t="str">
-        <v>6/24/2018</v>
+        <v>2018-06-23T18:30:00.000Z</v>
       </c>
       <c r="D21" t="str">
         <v>9 Talisman Center</v>
@@ -861,6 +921,9 @@
       </c>
       <c r="G21">
         <v>287</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
       </c>
     </row>
     <row r="22">
@@ -868,10 +931,10 @@
         <v>21</v>
       </c>
       <c r="B22" t="str">
-        <v>7/1/2018</v>
+        <v>2018-06-30T18:30:00.000Z</v>
       </c>
       <c r="C22" t="str">
-        <v>5/10/2018</v>
+        <v>2018-05-09T18:30:00.000Z</v>
       </c>
       <c r="D22" t="str">
         <v>44 Forest Drive</v>
@@ -884,6 +947,9 @@
       </c>
       <c r="G22">
         <v>474</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
       </c>
     </row>
     <row r="23">
@@ -891,10 +957,10 @@
         <v>22</v>
       </c>
       <c r="B23" t="str">
-        <v>1/25/2019</v>
+        <v>2019-01-24T18:30:00.000Z</v>
       </c>
       <c r="C23" t="str">
-        <v>6/19/2019</v>
+        <v>2019-06-18T18:30:00.000Z</v>
       </c>
       <c r="D23" t="str">
         <v>8 Nobel Avenue</v>
@@ -907,6 +973,9 @@
       </c>
       <c r="G23">
         <v>128</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
       </c>
     </row>
     <row r="24">
@@ -914,10 +983,10 @@
         <v>23</v>
       </c>
       <c r="B24" t="str">
-        <v>5/8/2018</v>
+        <v>2018-05-07T18:30:00.000Z</v>
       </c>
       <c r="C24" t="str">
-        <v>2/24/2019</v>
+        <v>2019-02-23T18:30:00.000Z</v>
       </c>
       <c r="D24" t="str">
         <v>1568 Carey Avenue</v>
@@ -930,6 +999,9 @@
       </c>
       <c r="G24">
         <v>464</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
       </c>
     </row>
     <row r="25">
@@ -937,10 +1009,10 @@
         <v>24</v>
       </c>
       <c r="B25" t="str">
-        <v>5/31/2018</v>
+        <v>2018-05-30T18:30:00.000Z</v>
       </c>
       <c r="C25" t="str">
-        <v>3/6/2019</v>
+        <v>2019-03-05T18:30:00.000Z</v>
       </c>
       <c r="D25" t="str">
         <v>99920 Lakewood Gardens Circle</v>
@@ -953,6 +1025,9 @@
       </c>
       <c r="G25">
         <v>193</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
       </c>
     </row>
     <row r="26">
@@ -960,10 +1035,10 @@
         <v>25</v>
       </c>
       <c r="B26" t="str">
-        <v>3/30/2019</v>
+        <v>2019-03-29T18:30:00.000Z</v>
       </c>
       <c r="C26" t="str">
-        <v>9/23/2018</v>
+        <v>2018-09-22T18:30:00.000Z</v>
       </c>
       <c r="D26" t="str">
         <v>80297 Del Mar Parkway</v>
@@ -976,6 +1051,9 @@
       </c>
       <c r="G26">
         <v>371</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
       </c>
     </row>
     <row r="27">
@@ -983,10 +1061,10 @@
         <v>26</v>
       </c>
       <c r="B27" t="str">
-        <v>10/31/2018</v>
+        <v>2018-10-30T18:30:00.000Z</v>
       </c>
       <c r="C27" t="str">
-        <v>4/6/2019</v>
+        <v>2019-04-05T18:30:00.000Z</v>
       </c>
       <c r="D27" t="str">
         <v>588 Riverside Lane</v>
@@ -999,6 +1077,9 @@
       </c>
       <c r="G27">
         <v>158</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
       </c>
     </row>
     <row r="28">
@@ -1006,10 +1087,10 @@
         <v>27</v>
       </c>
       <c r="B28" t="str">
-        <v>1/24/2018</v>
+        <v>2018-01-23T18:30:00.000Z</v>
       </c>
       <c r="C28" t="str">
-        <v>5/19/2019</v>
+        <v>2019-05-18T18:30:00.000Z</v>
       </c>
       <c r="D28" t="str">
         <v>3334 Reinke Circle</v>
@@ -1022,6 +1103,9 @@
       </c>
       <c r="G28">
         <v>328</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
       </c>
     </row>
     <row r="29">
@@ -1029,10 +1113,10 @@
         <v>28</v>
       </c>
       <c r="B29" t="str">
-        <v>6/17/2018</v>
+        <v>2018-06-16T18:30:00.000Z</v>
       </c>
       <c r="C29" t="str">
-        <v>9/4/2018</v>
+        <v>2018-09-03T18:30:00.000Z</v>
       </c>
       <c r="D29" t="str">
         <v>1 Katie Avenue</v>
@@ -1045,6 +1129,9 @@
       </c>
       <c r="G29">
         <v>93</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
       </c>
     </row>
     <row r="30">
@@ -1052,10 +1139,10 @@
         <v>29</v>
       </c>
       <c r="B30" t="str">
-        <v>9/22/2018</v>
+        <v>2018-09-21T18:30:00.000Z</v>
       </c>
       <c r="C30" t="str">
-        <v>1/15/2019</v>
+        <v>2019-01-14T18:30:00.000Z</v>
       </c>
       <c r="D30" t="str">
         <v>122 Express Hill</v>
@@ -1068,6 +1155,9 @@
       </c>
       <c r="G30">
         <v>194</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
       </c>
     </row>
     <row r="31">
@@ -1075,10 +1165,10 @@
         <v>30</v>
       </c>
       <c r="B31" t="str">
-        <v>5/15/2018</v>
+        <v>2018-05-14T18:30:00.000Z</v>
       </c>
       <c r="C31" t="str">
-        <v>12/29/2018</v>
+        <v>2018-12-28T18:30:00.000Z</v>
       </c>
       <c r="D31" t="str">
         <v>0311 Loomis Crossing</v>
@@ -1091,6 +1181,9 @@
       </c>
       <c r="G31">
         <v>222</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
       </c>
     </row>
     <row r="32">
@@ -1098,10 +1191,10 @@
         <v>31</v>
       </c>
       <c r="B32" t="str">
-        <v>11/9/2018</v>
+        <v>2018-11-08T18:30:00.000Z</v>
       </c>
       <c r="C32" t="str">
-        <v>10/15/2018</v>
+        <v>2018-10-14T18:30:00.000Z</v>
       </c>
       <c r="D32" t="str">
         <v>66 Melody Drive</v>
@@ -1114,6 +1207,9 @@
       </c>
       <c r="G32">
         <v>134</v>
+      </c>
+      <c r="H32">
+        <v>0</v>
       </c>
     </row>
     <row r="33">
@@ -1121,10 +1217,10 @@
         <v>32</v>
       </c>
       <c r="B33" t="str">
-        <v>5/6/2018</v>
+        <v>2018-05-05T18:30:00.000Z</v>
       </c>
       <c r="C33" t="str">
-        <v>11/19/2018</v>
+        <v>2018-11-18T18:30:00.000Z</v>
       </c>
       <c r="D33" t="str">
         <v>8688 Northfield Center</v>
@@ -1137,6 +1233,9 @@
       </c>
       <c r="G33">
         <v>451</v>
+      </c>
+      <c r="H33">
+        <v>0</v>
       </c>
     </row>
     <row r="34">
@@ -1144,10 +1243,10 @@
         <v>33</v>
       </c>
       <c r="B34" t="str">
-        <v>1/31/2018</v>
+        <v>2018-01-30T18:30:00.000Z</v>
       </c>
       <c r="C34" t="str">
-        <v>5/14/2019</v>
+        <v>2019-05-13T18:30:00.000Z</v>
       </c>
       <c r="D34" t="str">
         <v>9080 Comanche Circle</v>
@@ -1160,6 +1259,9 @@
       </c>
       <c r="G34">
         <v>178</v>
+      </c>
+      <c r="H34">
+        <v>0</v>
       </c>
     </row>
     <row r="35">
@@ -1167,10 +1269,10 @@
         <v>34</v>
       </c>
       <c r="B35" t="str">
-        <v>1/9/2019</v>
+        <v>2019-01-08T18:30:00.000Z</v>
       </c>
       <c r="C35" t="str">
-        <v>10/23/2018</v>
+        <v>2018-10-22T18:30:00.000Z</v>
       </c>
       <c r="D35" t="str">
         <v>39409 Pawling Park</v>
@@ -1183,6 +1285,9 @@
       </c>
       <c r="G35">
         <v>455</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
       </c>
     </row>
     <row r="36">
@@ -1190,10 +1295,10 @@
         <v>35</v>
       </c>
       <c r="B36" t="str">
-        <v>4/22/2018</v>
+        <v>2018-04-21T18:30:00.000Z</v>
       </c>
       <c r="C36" t="str">
-        <v>5/29/2019</v>
+        <v>2019-05-28T18:30:00.000Z</v>
       </c>
       <c r="D36" t="str">
         <v>823 New Castle Parkway</v>
@@ -1206,6 +1311,9 @@
       </c>
       <c r="G36">
         <v>78</v>
+      </c>
+      <c r="H36">
+        <v>0</v>
       </c>
     </row>
     <row r="37">
@@ -1213,10 +1321,10 @@
         <v>36</v>
       </c>
       <c r="B37" t="str">
-        <v>11/22/2018</v>
+        <v>2018-11-21T18:30:00.000Z</v>
       </c>
       <c r="C37" t="str">
-        <v>3/10/2019</v>
+        <v>2019-03-09T18:30:00.000Z</v>
       </c>
       <c r="D37" t="str">
         <v>4715 Londonderry Parkway</v>
@@ -1229,6 +1337,9 @@
       </c>
       <c r="G37">
         <v>72</v>
+      </c>
+      <c r="H37">
+        <v>0</v>
       </c>
     </row>
     <row r="38">
@@ -1236,10 +1347,10 @@
         <v>37</v>
       </c>
       <c r="B38" t="str">
-        <v>4/17/2018</v>
+        <v>2018-04-16T18:30:00.000Z</v>
       </c>
       <c r="C38" t="str">
-        <v>7/13/2018</v>
+        <v>2018-07-12T18:30:00.000Z</v>
       </c>
       <c r="D38" t="str">
         <v>998 Reinke Circle</v>
@@ -1252,6 +1363,9 @@
       </c>
       <c r="G38">
         <v>167</v>
+      </c>
+      <c r="H38">
+        <v>0</v>
       </c>
     </row>
     <row r="39">
@@ -1259,10 +1373,10 @@
         <v>38</v>
       </c>
       <c r="B39" t="str">
-        <v>8/6/2018</v>
+        <v>2018-08-05T18:30:00.000Z</v>
       </c>
       <c r="C39" t="str">
-        <v>7/7/2018</v>
+        <v>2018-07-06T18:30:00.000Z</v>
       </c>
       <c r="D39" t="str">
         <v>8 Sachs Street</v>
@@ -1275,6 +1389,9 @@
       </c>
       <c r="G39">
         <v>497</v>
+      </c>
+      <c r="H39">
+        <v>0</v>
       </c>
     </row>
     <row r="40">
@@ -1282,10 +1399,10 @@
         <v>39</v>
       </c>
       <c r="B40" t="str">
-        <v>7/20/2018</v>
+        <v>2018-07-19T18:30:00.000Z</v>
       </c>
       <c r="C40" t="str">
-        <v>4/11/2018</v>
+        <v>2018-04-10T18:30:00.000Z</v>
       </c>
       <c r="D40" t="str">
         <v>2 Golden Leaf Pass</v>
@@ -1298,6 +1415,9 @@
       </c>
       <c r="G40">
         <v>121</v>
+      </c>
+      <c r="H40">
+        <v>0</v>
       </c>
     </row>
     <row r="41">
@@ -1305,10 +1425,10 @@
         <v>40</v>
       </c>
       <c r="B41" t="str">
-        <v>3/31/2019</v>
+        <v>2019-03-30T18:30:00.000Z</v>
       </c>
       <c r="C41" t="str">
-        <v>12/31/2018</v>
+        <v>2018-12-30T18:30:00.000Z</v>
       </c>
       <c r="D41" t="str">
         <v>83178 Almo Point</v>
@@ -1321,6 +1441,9 @@
       </c>
       <c r="G41">
         <v>275</v>
+      </c>
+      <c r="H41">
+        <v>0</v>
       </c>
     </row>
     <row r="42">
@@ -1328,10 +1451,10 @@
         <v>41</v>
       </c>
       <c r="B42" t="str">
-        <v>3/21/2018</v>
+        <v>2018-03-20T18:30:00.000Z</v>
       </c>
       <c r="C42" t="str">
-        <v>1/15/2019</v>
+        <v>2019-01-14T18:30:00.000Z</v>
       </c>
       <c r="D42" t="str">
         <v>533 Drewry Hill</v>
@@ -1344,6 +1467,9 @@
       </c>
       <c r="G42">
         <v>448</v>
+      </c>
+      <c r="H42">
+        <v>0</v>
       </c>
     </row>
     <row r="43">
@@ -1351,10 +1477,10 @@
         <v>42</v>
       </c>
       <c r="B43" t="str">
-        <v>12/31/2018</v>
+        <v>2018-12-30T18:30:00.000Z</v>
       </c>
       <c r="C43" t="str">
-        <v>12/13/2018</v>
+        <v>2018-12-12T18:30:00.000Z</v>
       </c>
       <c r="D43" t="str">
         <v>060 Old Gate Lane</v>
@@ -1367,6 +1493,9 @@
       </c>
       <c r="G43">
         <v>204</v>
+      </c>
+      <c r="H43">
+        <v>0</v>
       </c>
     </row>
     <row r="44">
@@ -1374,10 +1503,10 @@
         <v>43</v>
       </c>
       <c r="B44" t="str">
-        <v>9/23/2018</v>
+        <v>2018-09-22T18:30:00.000Z</v>
       </c>
       <c r="C44" t="str">
-        <v>7/3/2018</v>
+        <v>2018-07-02T18:30:00.000Z</v>
       </c>
       <c r="D44" t="str">
         <v>5 Pennsylvania Center</v>
@@ -1390,6 +1519,9 @@
       </c>
       <c r="G44">
         <v>212</v>
+      </c>
+      <c r="H44">
+        <v>0</v>
       </c>
     </row>
     <row r="45">
@@ -1397,10 +1529,10 @@
         <v>44</v>
       </c>
       <c r="B45" t="str">
-        <v>11/29/2018</v>
+        <v>2018-11-28T18:30:00.000Z</v>
       </c>
       <c r="C45" t="str">
-        <v>11/20/2018</v>
+        <v>2018-11-19T18:30:00.000Z</v>
       </c>
       <c r="D45" t="str">
         <v>05639 Spohn Circle</v>
@@ -1413,6 +1545,9 @@
       </c>
       <c r="G45">
         <v>452</v>
+      </c>
+      <c r="H45">
+        <v>0</v>
       </c>
     </row>
     <row r="46">
@@ -1420,10 +1555,10 @@
         <v>45</v>
       </c>
       <c r="B46" t="str">
-        <v>5/29/2018</v>
+        <v>2018-05-28T18:30:00.000Z</v>
       </c>
       <c r="C46" t="str">
-        <v>10/26/2018</v>
+        <v>2018-10-25T18:30:00.000Z</v>
       </c>
       <c r="D46" t="str">
         <v>04 Dorton Pass</v>
@@ -1436,6 +1571,9 @@
       </c>
       <c r="G46">
         <v>295</v>
+      </c>
+      <c r="H46">
+        <v>0</v>
       </c>
     </row>
     <row r="47">
@@ -1443,10 +1581,10 @@
         <v>46</v>
       </c>
       <c r="B47" t="str">
-        <v>11/1/2018</v>
+        <v>2018-10-31T18:30:00.000Z</v>
       </c>
       <c r="C47" t="str">
-        <v>5/25/2019</v>
+        <v>2019-05-24T18:30:00.000Z</v>
       </c>
       <c r="D47" t="str">
         <v>16855 Graedel Street</v>
@@ -1459,6 +1597,9 @@
       </c>
       <c r="G47">
         <v>207</v>
+      </c>
+      <c r="H47">
+        <v>0</v>
       </c>
     </row>
     <row r="48">
@@ -1466,10 +1607,10 @@
         <v>47</v>
       </c>
       <c r="B48" t="str">
-        <v>1/26/2019</v>
+        <v>2019-01-25T18:30:00.000Z</v>
       </c>
       <c r="C48" t="str">
-        <v>9/3/2018</v>
+        <v>2018-09-02T18:30:00.000Z</v>
       </c>
       <c r="D48" t="str">
         <v>526 Banding Road</v>
@@ -1482,6 +1623,9 @@
       </c>
       <c r="G48">
         <v>380</v>
+      </c>
+      <c r="H48">
+        <v>0</v>
       </c>
     </row>
     <row r="49">
@@ -1489,10 +1633,10 @@
         <v>48</v>
       </c>
       <c r="B49" t="str">
-        <v>2/8/2019</v>
+        <v>2019-02-07T18:30:00.000Z</v>
       </c>
       <c r="C49" t="str">
-        <v>4/22/2019</v>
+        <v>2019-04-21T18:30:00.000Z</v>
       </c>
       <c r="D49" t="str">
         <v>3012 Merry Drive</v>
@@ -1505,6 +1649,9 @@
       </c>
       <c r="G49">
         <v>278</v>
+      </c>
+      <c r="H49">
+        <v>0</v>
       </c>
     </row>
     <row r="50">
@@ -1512,10 +1659,10 @@
         <v>49</v>
       </c>
       <c r="B50" t="str">
-        <v>11/7/2018</v>
+        <v>2018-11-06T18:30:00.000Z</v>
       </c>
       <c r="C50" t="str">
-        <v>7/29/2018</v>
+        <v>2018-07-28T18:30:00.000Z</v>
       </c>
       <c r="D50" t="str">
         <v>92454 Graedel Terrace</v>
@@ -1528,6 +1675,9 @@
       </c>
       <c r="G50">
         <v>110</v>
+      </c>
+      <c r="H50">
+        <v>0</v>
       </c>
     </row>
     <row r="51">
@@ -1535,10 +1685,10 @@
         <v>50</v>
       </c>
       <c r="B51" t="str">
-        <v>3/22/2018</v>
+        <v>2018-03-21T18:30:00.000Z</v>
       </c>
       <c r="C51" t="str">
-        <v>11/10/2018</v>
+        <v>2018-11-09T18:30:00.000Z</v>
       </c>
       <c r="D51" t="str">
         <v>20117 Debra Parkway</v>
@@ -1551,6 +1701,9 @@
       </c>
       <c r="G51">
         <v>66</v>
+      </c>
+      <c r="H51">
+        <v>0</v>
       </c>
     </row>
     <row r="52">
@@ -1558,10 +1711,10 @@
         <v>51</v>
       </c>
       <c r="B52" t="str">
-        <v>12/25/2018</v>
+        <v>2018-12-24T18:30:00.000Z</v>
       </c>
       <c r="C52" t="str">
-        <v>12/4/2018</v>
+        <v>2018-12-03T18:30:00.000Z</v>
       </c>
       <c r="D52" t="str">
         <v>2 Sutteridge Trail</v>
@@ -1574,6 +1727,9 @@
       </c>
       <c r="G52">
         <v>250</v>
+      </c>
+      <c r="H52">
+        <v>0</v>
       </c>
     </row>
     <row r="53">
@@ -1581,10 +1737,10 @@
         <v>52</v>
       </c>
       <c r="B53" t="str">
-        <v>5/1/2018</v>
+        <v>2018-04-30T18:30:00.000Z</v>
       </c>
       <c r="C53" t="str">
-        <v>6/8/2019</v>
+        <v>2019-06-07T18:30:00.000Z</v>
       </c>
       <c r="D53" t="str">
         <v>21166 Brown Way</v>
@@ -1597,6 +1753,9 @@
       </c>
       <c r="G53">
         <v>173</v>
+      </c>
+      <c r="H53">
+        <v>0</v>
       </c>
     </row>
     <row r="54">
@@ -1604,10 +1763,10 @@
         <v>53</v>
       </c>
       <c r="B54" t="str">
-        <v>10/5/2018</v>
+        <v>2018-10-04T18:30:00.000Z</v>
       </c>
       <c r="C54" t="str">
-        <v>6/13/2019</v>
+        <v>2019-06-12T18:30:00.000Z</v>
       </c>
       <c r="D54" t="str">
         <v>6752 Monterey Alley</v>
@@ -1620,6 +1779,9 @@
       </c>
       <c r="G54">
         <v>64</v>
+      </c>
+      <c r="H54">
+        <v>0</v>
       </c>
     </row>
     <row r="55">
@@ -1627,10 +1789,10 @@
         <v>54</v>
       </c>
       <c r="B55" t="str">
-        <v>8/31/2018</v>
+        <v>2018-08-30T18:30:00.000Z</v>
       </c>
       <c r="C55" t="str">
-        <v>1/4/2019</v>
+        <v>2019-01-03T18:30:00.000Z</v>
       </c>
       <c r="D55" t="str">
         <v>1345 Buell Place</v>
@@ -1643,6 +1805,9 @@
       </c>
       <c r="G55">
         <v>136</v>
+      </c>
+      <c r="H55">
+        <v>0</v>
       </c>
     </row>
     <row r="56">
@@ -1650,10 +1815,10 @@
         <v>55</v>
       </c>
       <c r="B56" t="str">
-        <v>7/10/2018</v>
+        <v>2018-07-09T18:30:00.000Z</v>
       </c>
       <c r="C56" t="str">
-        <v>11/12/2018</v>
+        <v>2018-11-11T18:30:00.000Z</v>
       </c>
       <c r="D56" t="str">
         <v>121 Alpine Lane</v>
@@ -1666,6 +1831,9 @@
       </c>
       <c r="G56">
         <v>118</v>
+      </c>
+      <c r="H56">
+        <v>0</v>
       </c>
     </row>
     <row r="57">
@@ -1673,10 +1841,10 @@
         <v>56</v>
       </c>
       <c r="B57" t="str">
-        <v>1/8/2018</v>
+        <v>2018-01-07T18:30:00.000Z</v>
       </c>
       <c r="C57" t="str">
-        <v>6/1/2018</v>
+        <v>2018-05-31T18:30:00.000Z</v>
       </c>
       <c r="D57" t="str">
         <v>2782 Dovetail Trail</v>
@@ -1689,6 +1857,9 @@
       </c>
       <c r="G57">
         <v>92</v>
+      </c>
+      <c r="H57">
+        <v>0</v>
       </c>
     </row>
     <row r="58">
@@ -1696,10 +1867,10 @@
         <v>57</v>
       </c>
       <c r="B58" t="str">
-        <v>6/8/2018</v>
+        <v>2018-06-07T18:30:00.000Z</v>
       </c>
       <c r="C58" t="str">
-        <v>2/13/2019</v>
+        <v>2019-02-12T18:30:00.000Z</v>
       </c>
       <c r="D58" t="str">
         <v>57 Almo Street</v>
@@ -1712,6 +1883,9 @@
       </c>
       <c r="G58">
         <v>126</v>
+      </c>
+      <c r="H58">
+        <v>0</v>
       </c>
     </row>
     <row r="59">
@@ -1719,10 +1893,10 @@
         <v>58</v>
       </c>
       <c r="B59" t="str">
-        <v>1/14/2019</v>
+        <v>2019-01-13T18:30:00.000Z</v>
       </c>
       <c r="C59" t="str">
-        <v>11/6/2018</v>
+        <v>2018-11-05T18:30:00.000Z</v>
       </c>
       <c r="D59" t="str">
         <v>825 Village Green Plaza</v>
@@ -1735,6 +1909,9 @@
       </c>
       <c r="G59">
         <v>330</v>
+      </c>
+      <c r="H59">
+        <v>0</v>
       </c>
     </row>
     <row r="60">
@@ -1742,10 +1919,10 @@
         <v>59</v>
       </c>
       <c r="B60" t="str">
-        <v>2/6/2019</v>
+        <v>2019-02-05T18:30:00.000Z</v>
       </c>
       <c r="C60" t="str">
-        <v>8/4/2018</v>
+        <v>2018-08-03T18:30:00.000Z</v>
       </c>
       <c r="D60" t="str">
         <v>419 Menomonie Place</v>
@@ -1758,6 +1935,9 @@
       </c>
       <c r="G60">
         <v>153</v>
+      </c>
+      <c r="H60">
+        <v>0</v>
       </c>
     </row>
     <row r="61">
@@ -1765,10 +1945,10 @@
         <v>60</v>
       </c>
       <c r="B61" t="str">
-        <v>1/14/2019</v>
+        <v>2019-01-13T18:30:00.000Z</v>
       </c>
       <c r="C61" t="str">
-        <v>6/23/2018</v>
+        <v>2018-06-22T18:30:00.000Z</v>
       </c>
       <c r="D61" t="str">
         <v>531 Nevada Hill</v>
@@ -1781,6 +1961,9 @@
       </c>
       <c r="G61">
         <v>290</v>
+      </c>
+      <c r="H61">
+        <v>0</v>
       </c>
     </row>
     <row r="62">
@@ -1788,10 +1971,10 @@
         <v>61</v>
       </c>
       <c r="B62" t="str">
-        <v>1/21/2018</v>
+        <v>2018-01-20T18:30:00.000Z</v>
       </c>
       <c r="C62" t="str">
-        <v>5/6/2019</v>
+        <v>2019-05-05T18:30:00.000Z</v>
       </c>
       <c r="D62" t="str">
         <v>135 Hoffman Plaza</v>
@@ -1804,6 +1987,9 @@
       </c>
       <c r="G62">
         <v>131</v>
+      </c>
+      <c r="H62">
+        <v>0</v>
       </c>
     </row>
     <row r="63">
@@ -1811,10 +1997,10 @@
         <v>62</v>
       </c>
       <c r="B63" t="str">
-        <v>5/27/2018</v>
+        <v>2018-05-26T18:30:00.000Z</v>
       </c>
       <c r="C63" t="str">
-        <v>8/26/2018</v>
+        <v>2018-08-25T18:30:00.000Z</v>
       </c>
       <c r="D63" t="str">
         <v>26 Hanover Parkway</v>
@@ -1827,6 +2013,9 @@
       </c>
       <c r="G63">
         <v>494</v>
+      </c>
+      <c r="H63">
+        <v>0</v>
       </c>
     </row>
     <row r="64">
@@ -1834,10 +2023,10 @@
         <v>63</v>
       </c>
       <c r="B64" t="str">
-        <v>9/23/2018</v>
+        <v>2018-09-22T18:30:00.000Z</v>
       </c>
       <c r="C64" t="str">
-        <v>8/6/2018</v>
+        <v>2018-08-05T18:30:00.000Z</v>
       </c>
       <c r="D64" t="str">
         <v>2 Cardinal Parkway</v>
@@ -1850,6 +2039,9 @@
       </c>
       <c r="G64">
         <v>353</v>
+      </c>
+      <c r="H64">
+        <v>0</v>
       </c>
     </row>
     <row r="65">
@@ -1857,10 +2049,10 @@
         <v>64</v>
       </c>
       <c r="B65" t="str">
-        <v>11/13/2018</v>
+        <v>2018-11-12T18:30:00.000Z</v>
       </c>
       <c r="C65" t="str">
-        <v>5/25/2019</v>
+        <v>2019-05-24T18:30:00.000Z</v>
       </c>
       <c r="D65" t="str">
         <v>94 Forster Center</v>
@@ -1873,6 +2065,9 @@
       </c>
       <c r="G65">
         <v>124</v>
+      </c>
+      <c r="H65">
+        <v>0</v>
       </c>
     </row>
     <row r="66">
@@ -1880,10 +2075,10 @@
         <v>65</v>
       </c>
       <c r="B66" t="str">
-        <v>6/15/2018</v>
+        <v>2018-06-14T18:30:00.000Z</v>
       </c>
       <c r="C66" t="str">
-        <v>8/12/2018</v>
+        <v>2018-08-11T18:30:00.000Z</v>
       </c>
       <c r="D66" t="str">
         <v>7945 Gerald Court</v>
@@ -1896,6 +2091,9 @@
       </c>
       <c r="G66">
         <v>58</v>
+      </c>
+      <c r="H66">
+        <v>0</v>
       </c>
     </row>
     <row r="67">
@@ -1903,10 +2101,10 @@
         <v>66</v>
       </c>
       <c r="B67" t="str">
-        <v>6/8/2018</v>
+        <v>2018-06-07T18:30:00.000Z</v>
       </c>
       <c r="C67" t="str">
-        <v>8/12/2018</v>
+        <v>2018-08-11T18:30:00.000Z</v>
       </c>
       <c r="D67" t="str">
         <v>66 Buhler Terrace</v>
@@ -1919,6 +2117,9 @@
       </c>
       <c r="G67">
         <v>316</v>
+      </c>
+      <c r="H67">
+        <v>0</v>
       </c>
     </row>
     <row r="68">
@@ -1926,10 +2127,10 @@
         <v>67</v>
       </c>
       <c r="B68" t="str">
-        <v>6/3/2018</v>
+        <v>2018-06-02T18:30:00.000Z</v>
       </c>
       <c r="C68" t="str">
-        <v>1/1/2019</v>
+        <v>2018-12-31T18:30:00.000Z</v>
       </c>
       <c r="D68" t="str">
         <v>5 Raven Trail</v>
@@ -1942,6 +2143,9 @@
       </c>
       <c r="G68">
         <v>379</v>
+      </c>
+      <c r="H68">
+        <v>0</v>
       </c>
     </row>
     <row r="69">
@@ -1949,10 +2153,10 @@
         <v>68</v>
       </c>
       <c r="B69" t="str">
-        <v>10/4/2018</v>
+        <v>2018-10-03T18:30:00.000Z</v>
       </c>
       <c r="C69" t="str">
-        <v>2/28/2019</v>
+        <v>2019-02-27T18:30:00.000Z</v>
       </c>
       <c r="D69" t="str">
         <v>31234 Garrison Hill</v>
@@ -1965,6 +2169,9 @@
       </c>
       <c r="G69">
         <v>137</v>
+      </c>
+      <c r="H69">
+        <v>0</v>
       </c>
     </row>
     <row r="70">
@@ -1972,10 +2179,10 @@
         <v>69</v>
       </c>
       <c r="B70" t="str">
-        <v>1/30/2018</v>
+        <v>2018-01-29T18:30:00.000Z</v>
       </c>
       <c r="C70" t="str">
-        <v>11/29/2018</v>
+        <v>2018-11-28T18:30:00.000Z</v>
       </c>
       <c r="D70" t="str">
         <v>30 Mosinee Way</v>
@@ -1988,6 +2195,9 @@
       </c>
       <c r="G70">
         <v>465</v>
+      </c>
+      <c r="H70">
+        <v>0</v>
       </c>
     </row>
     <row r="71">
@@ -1995,10 +2205,10 @@
         <v>70</v>
       </c>
       <c r="B71" t="str">
-        <v>2/18/2019</v>
+        <v>2019-02-17T18:30:00.000Z</v>
       </c>
       <c r="C71" t="str">
-        <v>7/8/2018</v>
+        <v>2018-07-07T18:30:00.000Z</v>
       </c>
       <c r="D71" t="str">
         <v>89 Vera Hill</v>
@@ -2011,6 +2221,9 @@
       </c>
       <c r="G71">
         <v>78</v>
+      </c>
+      <c r="H71">
+        <v>0</v>
       </c>
     </row>
     <row r="72">
@@ -2018,10 +2231,10 @@
         <v>71</v>
       </c>
       <c r="B72" t="str">
-        <v>7/24/2018</v>
+        <v>2018-07-23T18:30:00.000Z</v>
       </c>
       <c r="C72" t="str">
-        <v>9/18/2018</v>
+        <v>2018-09-17T18:30:00.000Z</v>
       </c>
       <c r="D72" t="str">
         <v>5669 Moland Terrace</v>
@@ -2034,6 +2247,9 @@
       </c>
       <c r="G72">
         <v>173</v>
+      </c>
+      <c r="H72">
+        <v>0</v>
       </c>
     </row>
     <row r="73">
@@ -2041,10 +2257,10 @@
         <v>72</v>
       </c>
       <c r="B73" t="str">
-        <v>3/24/2018</v>
+        <v>2018-03-23T18:30:00.000Z</v>
       </c>
       <c r="C73" t="str">
-        <v>2/18/2019</v>
+        <v>2019-02-17T18:30:00.000Z</v>
       </c>
       <c r="D73" t="str">
         <v>82341 Fallview Court</v>
@@ -2057,6 +2273,9 @@
       </c>
       <c r="G73">
         <v>266</v>
+      </c>
+      <c r="H73">
+        <v>0</v>
       </c>
     </row>
     <row r="74">
@@ -2064,10 +2283,10 @@
         <v>73</v>
       </c>
       <c r="B74" t="str">
-        <v>5/1/2018</v>
+        <v>2018-04-30T18:30:00.000Z</v>
       </c>
       <c r="C74" t="str">
-        <v>9/12/2018</v>
+        <v>2018-09-11T18:30:00.000Z</v>
       </c>
       <c r="D74" t="str">
         <v>9938 Homewood Parkway</v>
@@ -2080,6 +2299,9 @@
       </c>
       <c r="G74">
         <v>110</v>
+      </c>
+      <c r="H74">
+        <v>0</v>
       </c>
     </row>
     <row r="75">
@@ -2087,10 +2309,10 @@
         <v>74</v>
       </c>
       <c r="B75" t="str">
-        <v>3/1/2018</v>
+        <v>2018-02-28T18:30:00.000Z</v>
       </c>
       <c r="C75" t="str">
-        <v>3/31/2019</v>
+        <v>2019-03-30T18:30:00.000Z</v>
       </c>
       <c r="D75" t="str">
         <v>28 Chinook Terrace</v>
@@ -2103,6 +2325,9 @@
       </c>
       <c r="G75">
         <v>379</v>
+      </c>
+      <c r="H75">
+        <v>0</v>
       </c>
     </row>
     <row r="76">
@@ -2110,10 +2335,10 @@
         <v>75</v>
       </c>
       <c r="B76" t="str">
-        <v>3/19/2019</v>
+        <v>2019-03-18T18:30:00.000Z</v>
       </c>
       <c r="C76" t="str">
-        <v>10/7/2018</v>
+        <v>2018-10-06T18:30:00.000Z</v>
       </c>
       <c r="D76" t="str">
         <v>1 Sachtjen Terrace</v>
@@ -2126,6 +2351,9 @@
       </c>
       <c r="G76">
         <v>470</v>
+      </c>
+      <c r="H76">
+        <v>0</v>
       </c>
     </row>
     <row r="77">
@@ -2133,10 +2361,10 @@
         <v>76</v>
       </c>
       <c r="B77" t="str">
-        <v>11/16/2018</v>
+        <v>2018-11-15T18:30:00.000Z</v>
       </c>
       <c r="C77" t="str">
-        <v>6/17/2018</v>
+        <v>2018-06-16T18:30:00.000Z</v>
       </c>
       <c r="D77" t="str">
         <v>02 Fieldstone Court</v>
@@ -2149,6 +2377,9 @@
       </c>
       <c r="G77">
         <v>142</v>
+      </c>
+      <c r="H77">
+        <v>0</v>
       </c>
     </row>
     <row r="78">
@@ -2156,10 +2387,10 @@
         <v>77</v>
       </c>
       <c r="B78" t="str">
-        <v>12/27/2018</v>
+        <v>2018-12-26T18:30:00.000Z</v>
       </c>
       <c r="C78" t="str">
-        <v>1/8/2019</v>
+        <v>2019-01-07T18:30:00.000Z</v>
       </c>
       <c r="D78" t="str">
         <v>44 Old Shore Trail</v>
@@ -2172,6 +2403,9 @@
       </c>
       <c r="G78">
         <v>116</v>
+      </c>
+      <c r="H78">
+        <v>0</v>
       </c>
     </row>
     <row r="79">
@@ -2179,10 +2413,10 @@
         <v>78</v>
       </c>
       <c r="B79" t="str">
-        <v>3/1/2018</v>
+        <v>2018-02-28T18:30:00.000Z</v>
       </c>
       <c r="C79" t="str">
-        <v>9/5/2018</v>
+        <v>2018-09-04T18:30:00.000Z</v>
       </c>
       <c r="D79" t="str">
         <v>239 Grim Terrace</v>
@@ -2195,6 +2429,9 @@
       </c>
       <c r="G79">
         <v>308</v>
+      </c>
+      <c r="H79">
+        <v>0</v>
       </c>
     </row>
     <row r="80">
@@ -2202,10 +2439,10 @@
         <v>79</v>
       </c>
       <c r="B80" t="str">
-        <v>3/14/2018</v>
+        <v>2018-03-13T18:30:00.000Z</v>
       </c>
       <c r="C80" t="str">
-        <v>3/21/2019</v>
+        <v>2019-03-20T18:30:00.000Z</v>
       </c>
       <c r="D80" t="str">
         <v>86406 Quincy Court</v>
@@ -2218,6 +2455,9 @@
       </c>
       <c r="G80">
         <v>449</v>
+      </c>
+      <c r="H80">
+        <v>0</v>
       </c>
     </row>
     <row r="81">
@@ -2225,10 +2465,10 @@
         <v>80</v>
       </c>
       <c r="B81" t="str">
-        <v>7/25/2018</v>
+        <v>2018-07-24T18:30:00.000Z</v>
       </c>
       <c r="C81" t="str">
-        <v>2/2/2019</v>
+        <v>2019-02-01T18:30:00.000Z</v>
       </c>
       <c r="D81" t="str">
         <v>958 Grover Park</v>
@@ -2241,6 +2481,9 @@
       </c>
       <c r="G81">
         <v>287</v>
+      </c>
+      <c r="H81">
+        <v>0</v>
       </c>
     </row>
     <row r="82">
@@ -2248,10 +2491,10 @@
         <v>81</v>
       </c>
       <c r="B82" t="str">
-        <v>1/31/2018</v>
+        <v>2018-01-30T18:30:00.000Z</v>
       </c>
       <c r="C82" t="str">
-        <v>5/29/2018</v>
+        <v>2018-05-28T18:30:00.000Z</v>
       </c>
       <c r="D82" t="str">
         <v>9 Buhler Court</v>
@@ -2264,6 +2507,9 @@
       </c>
       <c r="G82">
         <v>67</v>
+      </c>
+      <c r="H82">
+        <v>0</v>
       </c>
     </row>
     <row r="83">
@@ -2271,10 +2517,10 @@
         <v>82</v>
       </c>
       <c r="B83" t="str">
-        <v>10/9/2018</v>
+        <v>2018-10-08T18:30:00.000Z</v>
       </c>
       <c r="C83" t="str">
-        <v>6/6/2018</v>
+        <v>2018-06-05T18:30:00.000Z</v>
       </c>
       <c r="D83" t="str">
         <v>41994 Oneill Hill</v>
@@ -2287,6 +2533,9 @@
       </c>
       <c r="G83">
         <v>444</v>
+      </c>
+      <c r="H83">
+        <v>0</v>
       </c>
     </row>
     <row r="84">
@@ -2294,10 +2543,10 @@
         <v>83</v>
       </c>
       <c r="B84" t="str">
-        <v>3/15/2019</v>
+        <v>2019-03-14T18:30:00.000Z</v>
       </c>
       <c r="C84" t="str">
-        <v>6/4/2019</v>
+        <v>2019-06-03T18:30:00.000Z</v>
       </c>
       <c r="D84" t="str">
         <v>245 Amoth Lane</v>
@@ -2310,6 +2559,9 @@
       </c>
       <c r="G84">
         <v>315</v>
+      </c>
+      <c r="H84">
+        <v>0</v>
       </c>
     </row>
     <row r="85">
@@ -2317,10 +2569,10 @@
         <v>84</v>
       </c>
       <c r="B85" t="str">
-        <v>2/6/2019</v>
+        <v>2019-02-05T18:30:00.000Z</v>
       </c>
       <c r="C85" t="str">
-        <v>6/19/2018</v>
+        <v>2018-06-18T18:30:00.000Z</v>
       </c>
       <c r="D85" t="str">
         <v>2380 Loeprich Street</v>
@@ -2333,6 +2585,9 @@
       </c>
       <c r="G85">
         <v>263</v>
+      </c>
+      <c r="H85">
+        <v>0</v>
       </c>
     </row>
     <row r="86">
@@ -2340,10 +2595,10 @@
         <v>85</v>
       </c>
       <c r="B86" t="str">
-        <v>8/5/2018</v>
+        <v>2018-08-04T18:30:00.000Z</v>
       </c>
       <c r="C86" t="str">
-        <v>4/17/2018</v>
+        <v>2018-04-16T18:30:00.000Z</v>
       </c>
       <c r="D86" t="str">
         <v>570 Artisan Crossing</v>
@@ -2356,6 +2611,9 @@
       </c>
       <c r="G86">
         <v>371</v>
+      </c>
+      <c r="H86">
+        <v>0</v>
       </c>
     </row>
     <row r="87">
@@ -2363,10 +2621,10 @@
         <v>86</v>
       </c>
       <c r="B87" t="str">
-        <v>1/9/2018</v>
+        <v>2018-01-08T18:30:00.000Z</v>
       </c>
       <c r="C87" t="str">
-        <v>9/27/2018</v>
+        <v>2018-09-26T18:30:00.000Z</v>
       </c>
       <c r="D87" t="str">
         <v>833 Buena Vista Court</v>
@@ -2379,6 +2637,9 @@
       </c>
       <c r="G87">
         <v>260</v>
+      </c>
+      <c r="H87">
+        <v>0</v>
       </c>
     </row>
     <row r="88">
@@ -2386,10 +2647,10 @@
         <v>87</v>
       </c>
       <c r="B88" t="str">
-        <v>9/27/2018</v>
+        <v>2018-09-26T18:30:00.000Z</v>
       </c>
       <c r="C88" t="str">
-        <v>10/21/2018</v>
+        <v>2018-10-20T18:30:00.000Z</v>
       </c>
       <c r="D88" t="str">
         <v>0501 Glendale Parkway</v>
@@ -2402,6 +2663,9 @@
       </c>
       <c r="G88">
         <v>76</v>
+      </c>
+      <c r="H88">
+        <v>0</v>
       </c>
     </row>
     <row r="89">
@@ -2409,10 +2673,10 @@
         <v>88</v>
       </c>
       <c r="B89" t="str">
-        <v>3/21/2018</v>
+        <v>2018-03-20T18:30:00.000Z</v>
       </c>
       <c r="C89" t="str">
-        <v>6/7/2018</v>
+        <v>2018-06-06T18:30:00.000Z</v>
       </c>
       <c r="D89" t="str">
         <v>1451 Scofield Parkway</v>
@@ -2425,6 +2689,9 @@
       </c>
       <c r="G89">
         <v>477</v>
+      </c>
+      <c r="H89">
+        <v>0</v>
       </c>
     </row>
     <row r="90">
@@ -2432,10 +2699,10 @@
         <v>89</v>
       </c>
       <c r="B90" t="str">
-        <v>8/6/2018</v>
+        <v>2018-08-05T18:30:00.000Z</v>
       </c>
       <c r="C90" t="str">
-        <v>3/4/2019</v>
+        <v>2019-03-03T18:30:00.000Z</v>
       </c>
       <c r="D90" t="str">
         <v>92 Farwell Court</v>
@@ -2448,6 +2715,9 @@
       </c>
       <c r="G90">
         <v>85</v>
+      </c>
+      <c r="H90">
+        <v>0</v>
       </c>
     </row>
     <row r="91">
@@ -2455,10 +2725,10 @@
         <v>90</v>
       </c>
       <c r="B91" t="str">
-        <v>3/27/2019</v>
+        <v>2019-03-26T18:30:00.000Z</v>
       </c>
       <c r="C91" t="str">
-        <v>1/13/2019</v>
+        <v>2019-01-12T18:30:00.000Z</v>
       </c>
       <c r="D91" t="str">
         <v>66162 Division Trail</v>
@@ -2471,6 +2741,9 @@
       </c>
       <c r="G91">
         <v>428</v>
+      </c>
+      <c r="H91">
+        <v>0</v>
       </c>
     </row>
     <row r="92">
@@ -2478,10 +2751,10 @@
         <v>91</v>
       </c>
       <c r="B92" t="str">
-        <v>7/27/2018</v>
+        <v>2018-07-26T18:30:00.000Z</v>
       </c>
       <c r="C92" t="str">
-        <v>5/17/2018</v>
+        <v>2018-05-16T18:30:00.000Z</v>
       </c>
       <c r="D92" t="str">
         <v>1 Bellgrove Road</v>
@@ -2494,6 +2767,9 @@
       </c>
       <c r="G92">
         <v>201</v>
+      </c>
+      <c r="H92">
+        <v>0</v>
       </c>
     </row>
     <row r="93">
@@ -2501,10 +2777,10 @@
         <v>92</v>
       </c>
       <c r="B93" t="str">
-        <v>12/3/2018</v>
+        <v>2018-12-02T18:30:00.000Z</v>
       </c>
       <c r="C93" t="str">
-        <v>5/5/2019</v>
+        <v>2019-05-04T18:30:00.000Z</v>
       </c>
       <c r="D93" t="str">
         <v>41 Moose Crossing</v>
@@ -2517,6 +2793,9 @@
       </c>
       <c r="G93">
         <v>166</v>
+      </c>
+      <c r="H93">
+        <v>0</v>
       </c>
     </row>
     <row r="94">
@@ -2524,10 +2803,10 @@
         <v>93</v>
       </c>
       <c r="B94" t="str">
-        <v>7/9/2018</v>
+        <v>2018-07-08T18:30:00.000Z</v>
       </c>
       <c r="C94" t="str">
-        <v>12/22/2018</v>
+        <v>2018-12-21T18:30:00.000Z</v>
       </c>
       <c r="D94" t="str">
         <v>66214 Hoepker Circle</v>
@@ -2540,6 +2819,9 @@
       </c>
       <c r="G94">
         <v>189</v>
+      </c>
+      <c r="H94">
+        <v>0</v>
       </c>
     </row>
     <row r="95">
@@ -2547,10 +2829,10 @@
         <v>94</v>
       </c>
       <c r="B95" t="str">
-        <v>10/7/2018</v>
+        <v>2018-10-06T18:30:00.000Z</v>
       </c>
       <c r="C95" t="str">
-        <v>4/13/2019</v>
+        <v>2019-04-12T18:30:00.000Z</v>
       </c>
       <c r="D95" t="str">
         <v>19 Linden Street</v>
@@ -2563,6 +2845,9 @@
       </c>
       <c r="G95">
         <v>453</v>
+      </c>
+      <c r="H95">
+        <v>0</v>
       </c>
     </row>
     <row r="96">
@@ -2570,10 +2855,10 @@
         <v>95</v>
       </c>
       <c r="B96" t="str">
-        <v>3/22/2018</v>
+        <v>2018-03-21T18:30:00.000Z</v>
       </c>
       <c r="C96" t="str">
-        <v>8/26/2018</v>
+        <v>2018-08-25T18:30:00.000Z</v>
       </c>
       <c r="D96" t="str">
         <v>84008 Debra Trail</v>
@@ -2586,6 +2871,9 @@
       </c>
       <c r="G96">
         <v>167</v>
+      </c>
+      <c r="H96">
+        <v>0</v>
       </c>
     </row>
     <row r="97">
@@ -2593,10 +2881,10 @@
         <v>96</v>
       </c>
       <c r="B97" t="str">
-        <v>10/13/2018</v>
+        <v>2018-10-12T18:30:00.000Z</v>
       </c>
       <c r="C97" t="str">
-        <v>6/2/2019</v>
+        <v>2019-06-01T18:30:00.000Z</v>
       </c>
       <c r="D97" t="str">
         <v>072 Golf Course Hill</v>
@@ -2609,6 +2897,9 @@
       </c>
       <c r="G97">
         <v>184</v>
+      </c>
+      <c r="H97">
+        <v>0</v>
       </c>
     </row>
     <row r="98">
@@ -2616,10 +2907,10 @@
         <v>97</v>
       </c>
       <c r="B98" t="str">
-        <v>10/13/2018</v>
+        <v>2018-10-12T18:30:00.000Z</v>
       </c>
       <c r="C98" t="str">
-        <v>9/24/2018</v>
+        <v>2018-09-23T18:30:00.000Z</v>
       </c>
       <c r="D98" t="str">
         <v>900 Maple Wood Crossing</v>
@@ -2632,6 +2923,9 @@
       </c>
       <c r="G98">
         <v>385</v>
+      </c>
+      <c r="H98">
+        <v>0</v>
       </c>
     </row>
     <row r="99">
@@ -2639,10 +2933,10 @@
         <v>98</v>
       </c>
       <c r="B99" t="str">
-        <v>3/10/2019</v>
+        <v>2019-03-09T18:30:00.000Z</v>
       </c>
       <c r="C99" t="str">
-        <v>4/23/2018</v>
+        <v>2018-04-22T18:30:00.000Z</v>
       </c>
       <c r="D99" t="str">
         <v>59 Maple Wood Point</v>
@@ -2655,6 +2949,9 @@
       </c>
       <c r="G99">
         <v>126</v>
+      </c>
+      <c r="H99">
+        <v>0</v>
       </c>
     </row>
     <row r="100">
@@ -2662,10 +2959,10 @@
         <v>99</v>
       </c>
       <c r="B100" t="str">
-        <v>4/19/2018</v>
+        <v>2018-04-18T18:30:00.000Z</v>
       </c>
       <c r="C100" t="str">
-        <v>4/8/2018</v>
+        <v>2018-04-07T18:30:00.000Z</v>
       </c>
       <c r="D100" t="str">
         <v>71991 Del Sol Way</v>
@@ -2678,6 +2975,9 @@
       </c>
       <c r="G100">
         <v>290</v>
+      </c>
+      <c r="H100">
+        <v>0</v>
       </c>
     </row>
     <row r="101">
@@ -2685,10 +2985,10 @@
         <v>100</v>
       </c>
       <c r="B101" t="str">
-        <v>5/21/2018</v>
+        <v>2018-05-20T18:30:00.000Z</v>
       </c>
       <c r="C101" t="str">
-        <v>5/14/2018</v>
+        <v>2018-05-13T18:30:00.000Z</v>
       </c>
       <c r="D101" t="str">
         <v>0743 Sutteridge Plaza</v>
@@ -2702,10 +3002,13 @@
       <c r="G101">
         <v>94</v>
       </c>
+      <c r="H101">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G101"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H101"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>